<commit_message>
ANIM UE5 MM anim ATK 1 / 2
</commit_message>
<xml_diff>
--- a/Documents/CombatSystem/EnemySheet.xlsx
+++ b/Documents/CombatSystem/EnemySheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameEngineWork\UNREAL\PFEURA\Documents\CombatSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian MAGNO\Desktop\PFEURA\Documents\CombatSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B54B7-531F-459D-B726-D5F609325261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450D600D-D0E1-4D78-BCC1-E2A83C57DB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,6 +284,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -291,12 +297,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,131 +583,131 @@
       <selection activeCell="J8" sqref="A7:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -878,10 +878,10 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="7" width="50.7109375" customWidth="1"/>
@@ -889,125 +889,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1042,16 +1042,16 @@
       <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1071,10 +1071,10 @@
       <c r="E12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>